<commit_message>
add libraries poi-3.17 xmlbeans-2.6.0 variable declaration of input data
</commit_message>
<xml_diff>
--- a/lorry.xlsx
+++ b/lorry.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
   <si>
     <t>Date</t>
   </si>
@@ -101,6 +101,9 @@
   </si>
   <si>
     <t>4564</t>
+  </si>
+  <si>
+    <t>14-03-2018</t>
   </si>
 </sst>
 </file>
@@ -454,7 +457,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K7" sqref="A2:K7"/>
@@ -817,6 +820,41 @@
         <v>13</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" t="n">
+        <v>56000.0</v>
+      </c>
+      <c r="D11" t="n">
+        <v>57000.0</v>
+      </c>
+      <c r="E11" t="n">
+        <v>8000.0</v>
+      </c>
+      <c r="F11" t="n">
+        <v>66.0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>150.0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J11" t="n">
+        <v>37600.0</v>
+      </c>
+      <c r="K11" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>